<commit_message>
incluido dados de nome social
</commit_message>
<xml_diff>
--- a/ANALISE/Tabelas Auxiliares.xlsx
+++ b/ANALISE/Tabelas Auxiliares.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandro Soares\Desktop\Enem_2019\ANALISE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3450D82-B59E-4425-A9EC-68CCEA2D99DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FABFE9-DF6B-4316-A56D-C5B965FCBB46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ITENS_PROVA_2019" sheetId="3" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="TIPO_ESCOLA" sheetId="7" r:id="rId14"/>
     <sheet name="REDAÇÃO" sheetId="9" r:id="rId15"/>
     <sheet name="LINGUAGEM_ESCOLHIDA" sheetId="10" r:id="rId16"/>
+    <sheet name="Nome_Social" sheetId="19" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="ESTADOS">Tabela3[#All]</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="584">
   <si>
     <t>NU_INSCRICAO</t>
   </si>
@@ -2572,6 +2573,21 @@
   </si>
   <si>
     <t>Renda Familiar</t>
+  </si>
+  <si>
+    <t>Possui</t>
+  </si>
+  <si>
+    <t>Não possui</t>
+  </si>
+  <si>
+    <t>Não Declarou</t>
+  </si>
+  <si>
+    <t>Declarou</t>
+  </si>
+  <si>
+    <t>Nome Social</t>
   </si>
 </sst>
 </file>
@@ -3335,6 +3351,17 @@
 </table>
 </file>
 
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{687139D9-AEB4-4000-8B21-7229268AAECB}" name="Tabela17" displayName="Tabela17" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{31DE32A3-27F1-4014-83D9-5B1AB31DA7F3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CD78C820-1EE9-4648-A633-00D4E44E9B19}" name="IN_NOME_SOCIAL"/>
+    <tableColumn id="2" xr3:uid="{C552CC24-3110-4FB9-BCFD-C005C4DC871B}" name="Nome Social"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{469627C8-F7E5-4223-9D8E-20D3A83FC4A1}" name="Tabela14" displayName="Tabela14" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3" xr:uid="{D4F824D6-C23C-4580-BB5A-C1FA1F154C15}"/>
@@ -4053,7 +4080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618AE0E5-51A7-4D36-B25B-25F830965FA3}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
@@ -4886,6 +4913,52 @@
       </c>
       <c r="B3" t="s">
         <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D160DBD9-CD88-4AA3-8C2E-F49FC3C260A6}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -13392,7 +13465,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13414,7 +13487,7 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -13422,7 +13495,7 @@
         <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>